<commit_message>
Made FilterMessageFileSource.describe() use only file name, not path
</commit_message>
<xml_diff>
--- a/src/test/resources/TestEndToEnd/AddSenders Expected Output.xlsx
+++ b/src/test/resources/TestEndToEnd/AddSenders Expected Output.xlsx
@@ -122,16 +122,16 @@
     <t>Ignored Patterns</t>
   </si>
   <si>
-    <t>src/test/resources/TestEndToEnd/To Be Unsubscribed.csv</t>
-  </si>
-  <si>
     <t>Personal Domains</t>
   </si>
   <si>
-    <t>src/test/resources/TestEndToEnd/Colleagues.csv</t>
-  </si>
-  <si>
     <t>AddSenderRule</t>
+  </si>
+  <si>
+    <t>To Be Unsubscribed.csv</t>
+  </si>
+  <si>
+    <t>Colleagues.csv</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -643,7 +643,7 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -683,7 +683,7 @@
         <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -703,7 +703,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -720,10 +720,10 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -740,10 +740,10 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -760,10 +760,10 @@
         <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -780,10 +780,10 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -800,10 +800,10 @@
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -820,10 +820,10 @@
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -843,7 +843,7 @@
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>